<commit_message>
Categories and features are updated
</commit_message>
<xml_diff>
--- a/auxiliary/categories.xlsx
+++ b/auxiliary/categories.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22905"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\41395550350ana\Desktop\aliyurekli\github\RecSys-MPD\auxiliary\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14685"/>
   </bookViews>
   <sheets>
     <sheet name="research" sheetId="2" r:id="rId1"/>
@@ -12,18 +17,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="28">
   <si>
     <t>CATEGORY NO</t>
   </si>
@@ -97,19 +102,22 @@
     <t>HOLDOUT RATIO</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>Half of the tracks are hidden, seeds are randomized</t>
+    <t>33% of the tracks are hidden, seeds are randomized</t>
+  </si>
+  <si>
+    <t>25% of the tracks are hidden, seeds are randomized</t>
+  </si>
+  <si>
+    <t>50% of the tracks are hidden, seeds are randomized</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,10 +199,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="İzlenen Köprü" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="İzlenen Köprü" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Köprü" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Köprü" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,7 +473,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -476,19 +484,19 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="47.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,25 +507,50 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>24</v>
+      <c r="B2" s="4">
+        <v>0.5</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0.33</v>
+      </c>
+      <c r="C3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="C4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -538,20 +571,20 @@
       <selection sqref="A1:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="18.5" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -580,7 +613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -609,7 +642,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -638,7 +671,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -667,7 +700,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -696,7 +729,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -725,7 +758,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -754,7 +787,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -783,7 +816,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -812,7 +845,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -841,7 +874,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>

</xml_diff>